<commit_message>
Mod2 access + Extended
</commit_message>
<xml_diff>
--- a/3-Optimize.xlsx
+++ b/3-Optimize.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC9C919-E86D-4F36-A688-684CA7C9EFF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B34DB3-66B7-4423-AB98-A1BAEFDA3CA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="160">
   <si>
     <t>Algorithm</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Number</t>
-  </si>
-  <si>
-    <t>Paramaeters</t>
   </si>
   <si>
     <t>Dataset</t>
@@ -948,51 +945,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1055,6 +1007,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -21577,8 +21574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z31" workbookViewId="0">
-      <selection activeCell="AG36" sqref="AG36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21614,87 +21611,87 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="88" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="95" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="92"/>
-      <c r="Z1" s="92"/>
-      <c r="AA1" s="92"/>
-      <c r="AB1" s="92"/>
-      <c r="AC1" s="82" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
-      <c r="AG1" s="83"/>
-      <c r="AH1" s="83"/>
-      <c r="AI1" s="83"/>
-      <c r="AJ1" s="83"/>
-      <c r="AK1" s="83"/>
-      <c r="AL1" s="83"/>
-      <c r="AM1" s="83"/>
-      <c r="AN1" s="83"/>
-      <c r="AO1" s="83"/>
-      <c r="AP1" s="83"/>
-      <c r="AQ1" s="84" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="68"/>
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="AR1" s="70"/>
+      <c r="AS1" s="70"/>
+      <c r="AT1" s="70"/>
+      <c r="AU1" s="70"/>
+      <c r="AV1" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="AR1" s="85"/>
-      <c r="AS1" s="85"/>
-      <c r="AT1" s="85"/>
-      <c r="AU1" s="85"/>
-      <c r="AV1" s="86" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
-      <c r="AY1" s="87"/>
-      <c r="AZ1" s="87"/>
-      <c r="BA1" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="BB1" s="80"/>
-      <c r="BC1" s="80"/>
-      <c r="BD1" s="80"/>
-      <c r="BE1" s="80"/>
-      <c r="BF1" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="BG1" s="78"/>
-      <c r="BH1" s="78"/>
-      <c r="BI1" s="78"/>
-      <c r="BJ1" s="78"/>
+      <c r="AW1" s="72"/>
+      <c r="AX1" s="72"/>
+      <c r="AY1" s="72"/>
+      <c r="AZ1" s="72"/>
+      <c r="BA1" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="65"/>
+      <c r="BC1" s="65"/>
+      <c r="BD1" s="65"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="BG1" s="63"/>
+      <c r="BH1" s="63"/>
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="63"/>
     </row>
     <row r="2" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
@@ -21705,186 +21702,186 @@
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="I2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="S2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="U2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="17" t="s">
-        <v>45</v>
-      </c>
       <c r="X2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Z2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="AA2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AB2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="17" t="s">
-        <v>52</v>
-      </c>
       <c r="AC2" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" s="28" t="s">
+      <c r="AE2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" s="28" t="s">
+      <c r="AF2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="AF2" s="28" t="s">
+      <c r="AG2" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AG2" s="28" t="s">
+      <c r="AH2" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="AH2" s="28" t="s">
+      <c r="AI2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" s="28" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="AJ2" s="28" t="s">
+      <c r="AK2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="28" t="s">
+      <c r="AL2" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="AL2" s="28" t="s">
-        <v>73</v>
-      </c>
       <c r="AM2" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN2" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="AN2" s="28" t="s">
+      <c r="AO2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="AO2" s="28" t="s">
+      <c r="AP2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" s="28" t="s">
-        <v>78</v>
-      </c>
       <c r="AQ2" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="AR2" s="32" t="s">
+      <c r="AS2" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="AS2" s="32" t="s">
+      <c r="AT2" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="AT2" s="32" t="s">
+      <c r="AU2" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="AU2" s="32" t="s">
+      <c r="AV2" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="AV2" s="33" t="s">
+      <c r="AW2" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="AW2" s="34" t="s">
+      <c r="AX2" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="AX2" s="34" t="s">
+      <c r="AY2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AY2" s="34" t="s">
+      <c r="AZ2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="AZ2" s="34" t="s">
-        <v>104</v>
-      </c>
       <c r="BA2" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="BB2" s="35" t="s">
+      <c r="BC2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="BC2" s="35" t="s">
+      <c r="BD2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="BD2" s="35" t="s">
+      <c r="BE2" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="BE2" s="35" t="s">
-        <v>112</v>
-      </c>
       <c r="BF2" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="BG2" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="BG2" s="38" t="s">
+      <c r="BH2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="BH2" s="38" t="s">
+      <c r="BI2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="BI2" s="38" t="s">
+      <c r="BJ2" s="38" t="s">
         <v>123</v>
-      </c>
-      <c r="BJ2" s="38" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
-        <v>23</v>
+      <c r="A3" s="85" t="s">
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -22130,7 +22127,7 @@
       </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
+      <c r="A4" s="86"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -22375,7 +22372,7 @@
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
+      <c r="A5" s="86"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -22620,7 +22617,7 @@
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -22865,8 +22862,8 @@
       </c>
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
-        <v>24</v>
+      <c r="A7" s="88" t="s">
+        <v>23</v>
       </c>
       <c r="B7" t="str">
         <f>B3</f>
@@ -23055,7 +23052,7 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
+      <c r="A8" s="86"/>
       <c r="B8" t="str">
         <f t="shared" ref="B8:C8" si="32">B4</f>
         <v>skopt.dummy_min</v>
@@ -23243,7 +23240,7 @@
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A9" s="67"/>
+      <c r="A9" s="86"/>
       <c r="B9" t="str">
         <f t="shared" ref="B9:C9" si="33">B5</f>
         <v>skopt.forest_min</v>
@@ -23431,7 +23428,7 @@
       </c>
     </row>
     <row r="10" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A10" s="68"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="1" t="str">
         <f t="shared" ref="B10:C10" si="34">B6</f>
         <v>skopt.gbrt_min</v>
@@ -23619,8 +23616,8 @@
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A11" s="69" t="s">
-        <v>25</v>
+      <c r="A11" s="88" t="s">
+        <v>24</v>
       </c>
       <c r="B11" t="str">
         <f>B3</f>
@@ -23809,7 +23806,7 @@
       </c>
     </row>
     <row r="12" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
+      <c r="A12" s="86"/>
       <c r="B12" t="str">
         <f t="shared" ref="B12:C12" si="35">B4</f>
         <v>skopt.dummy_min</v>
@@ -23997,7 +23994,7 @@
       </c>
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
+      <c r="A13" s="86"/>
       <c r="B13" t="str">
         <f t="shared" ref="B13:C13" si="36">B5</f>
         <v>skopt.forest_min</v>
@@ -24185,7 +24182,7 @@
       </c>
     </row>
     <row r="14" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A14" s="68"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="1" t="str">
         <f t="shared" ref="B14:C14" si="37">B6</f>
         <v>skopt.gbrt_min</v>
@@ -24373,8 +24370,8 @@
       </c>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A15" s="69" t="s">
-        <v>26</v>
+      <c r="A15" s="88" t="s">
+        <v>25</v>
       </c>
       <c r="B15" t="str">
         <f>B3</f>
@@ -24563,7 +24560,7 @@
       </c>
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
+      <c r="A16" s="86"/>
       <c r="B16" t="str">
         <f t="shared" ref="B16:C16" si="38">B4</f>
         <v>skopt.dummy_min</v>
@@ -24751,7 +24748,7 @@
       </c>
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A17" s="67"/>
+      <c r="A17" s="86"/>
       <c r="B17" t="str">
         <f t="shared" ref="B17:C17" si="39">B5</f>
         <v>skopt.forest_min</v>
@@ -24939,7 +24936,7 @@
       </c>
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="1" t="str">
         <f t="shared" ref="B18:C18" si="40">B6</f>
         <v>skopt.gbrt_min</v>
@@ -25127,8 +25124,8 @@
       </c>
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A19" s="69" t="s">
-        <v>27</v>
+      <c r="A19" s="88" t="s">
+        <v>26</v>
       </c>
       <c r="B19" t="str">
         <f>B3</f>
@@ -25317,7 +25314,7 @@
       </c>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
+      <c r="A20" s="86"/>
       <c r="B20" t="str">
         <f t="shared" ref="B20:C20" si="41">B4</f>
         <v>skopt.dummy_min</v>
@@ -25505,7 +25502,7 @@
       </c>
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
+      <c r="A21" s="86"/>
       <c r="B21" t="str">
         <f t="shared" ref="B21:C21" si="42">B5</f>
         <v>skopt.forest_min</v>
@@ -25693,7 +25690,7 @@
       </c>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A22" s="68"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="1" t="str">
         <f t="shared" ref="B22:C22" si="43">B6</f>
         <v>skopt.gbrt_min</v>
@@ -25881,8 +25878,8 @@
       </c>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A23" s="69" t="s">
-        <v>28</v>
+      <c r="A23" s="88" t="s">
+        <v>27</v>
       </c>
       <c r="B23" t="str">
         <f>B3</f>
@@ -26071,7 +26068,7 @@
       </c>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
+      <c r="A24" s="86"/>
       <c r="B24" t="str">
         <f t="shared" ref="B24:C24" si="44">B4</f>
         <v>skopt.dummy_min</v>
@@ -26259,7 +26256,7 @@
       </c>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
+      <c r="A25" s="86"/>
       <c r="B25" t="str">
         <f t="shared" ref="B25:C25" si="45">B5</f>
         <v>skopt.forest_min</v>
@@ -26447,7 +26444,7 @@
       </c>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
+      <c r="A26" s="86"/>
       <c r="B26" t="str">
         <f t="shared" ref="B26:C26" si="46">B6</f>
         <v>skopt.gbrt_min</v>
@@ -26652,10 +26649,10 @@
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AC28" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
@@ -26673,10 +26670,10 @@
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC29" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
@@ -26694,10 +26691,10 @@
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AC30" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
@@ -26733,202 +26730,202 @@
       <c r="A32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="70" t="s">
+      <c r="B32" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="93"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
+      <c r="O32" s="90"/>
+      <c r="P32" s="90"/>
+      <c r="Q32" s="90"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="92" t="s">
+        <v>125</v>
+      </c>
+      <c r="T32" s="92"/>
+      <c r="U32" s="92"/>
+      <c r="V32" s="92"/>
+      <c r="W32" s="92"/>
+      <c r="X32" s="92"/>
+      <c r="Y32" s="92"/>
+      <c r="Z32" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA32" s="83"/>
+      <c r="AB32" s="83"/>
+      <c r="AC32" s="83"/>
+      <c r="AD32" s="83"/>
+      <c r="AE32" s="83"/>
+      <c r="AF32" s="84"/>
+      <c r="AG32" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="71"/>
-      <c r="O32" s="71"/>
-      <c r="P32" s="71"/>
-      <c r="Q32" s="71"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="T32" s="73"/>
-      <c r="U32" s="73"/>
-      <c r="V32" s="73"/>
-      <c r="W32" s="73"/>
-      <c r="X32" s="73"/>
-      <c r="Y32" s="73"/>
-      <c r="Z32" s="63" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA32" s="64"/>
-      <c r="AB32" s="64"/>
-      <c r="AC32" s="64"/>
-      <c r="AD32" s="64"/>
-      <c r="AE32" s="64"/>
-      <c r="AF32" s="65"/>
-      <c r="AG32" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH32" s="76"/>
-      <c r="AI32" s="76"/>
-      <c r="AJ32" s="76"/>
-      <c r="AK32" s="76"/>
-      <c r="AL32" s="76"/>
-      <c r="AM32" s="76"/>
-      <c r="AN32" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="AO32" s="78"/>
-      <c r="AP32" s="78"/>
-      <c r="AQ32" s="78"/>
-      <c r="AR32" s="78"/>
-      <c r="AS32" s="78"/>
-      <c r="AT32" s="78"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="61"/>
+      <c r="AJ32" s="61"/>
+      <c r="AK32" s="61"/>
+      <c r="AL32" s="61"/>
+      <c r="AM32" s="61"/>
+      <c r="AN32" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="AO32" s="63"/>
+      <c r="AP32" s="63"/>
+      <c r="AQ32" s="63"/>
+      <c r="AR32" s="63"/>
+      <c r="AS32" s="63"/>
+      <c r="AT32" s="63"/>
     </row>
     <row r="33" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="51" t="s">
+      <c r="F33" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="52" t="s">
-        <v>14</v>
-      </c>
       <c r="G33" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="H33" s="54" t="s">
+      <c r="I33" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="54" t="s">
+      <c r="J33" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="54" t="s">
+      <c r="K33" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="54" t="s">
+      <c r="L33" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="L33" s="54" t="s">
+      <c r="M33" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="M33" s="54" t="s">
+      <c r="N33" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="O33" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="P33" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q33" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="R33" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="N33" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="O33" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="P33" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q33" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="R33" s="57" t="s">
-        <v>87</v>
-      </c>
       <c r="S33" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="T33" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="T33" s="5" t="s">
+      <c r="U33" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="U33" s="5" t="s">
+      <c r="V33" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="V33" s="5" t="s">
+      <c r="W33" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="W33" s="5" t="s">
+      <c r="X33" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="X33" s="5" t="s">
+      <c r="Y33" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="Y33" s="5" t="s">
+      <c r="Z33" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="Z33" s="55" t="s">
+      <c r="AA33" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="AA33" s="56" t="s">
+      <c r="AB33" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="AB33" s="56" t="s">
+      <c r="AC33" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="AC33" s="56" t="s">
+      <c r="AD33" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="AD33" s="56" t="s">
+      <c r="AE33" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="AE33" s="56" t="s">
+      <c r="AF33" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="AF33" s="58" t="s">
-        <v>141</v>
-      </c>
       <c r="AG33" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH33" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="AH33" s="60" t="s">
+      <c r="AI33" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="AI33" s="60" t="s">
+      <c r="AJ33" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="AJ33" s="60" t="s">
+      <c r="AK33" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="AK33" s="60" t="s">
+      <c r="AL33" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="AL33" s="60" t="s">
+      <c r="AM33" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="AM33" s="60" t="s">
+      <c r="AN33" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="AN33" s="38" t="s">
+      <c r="AO33" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="AO33" s="38" t="s">
+      <c r="AP33" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="AP33" s="38" t="s">
+      <c r="AQ33" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="AQ33" s="38" t="s">
+      <c r="AR33" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="AR33" s="38" t="s">
+      <c r="AS33" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="AS33" s="38" t="s">
+      <c r="AT33" s="38" t="s">
         <v>155</v>
-      </c>
-      <c r="AT33" s="38" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.3">
@@ -26936,10 +26933,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" s="12">
         <v>10</v>
@@ -27083,7 +27080,7 @@
         <v>20.005243465415532</v>
       </c>
       <c r="AV34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.3">
@@ -27091,10 +27088,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D35" s="12">
         <v>10</v>
@@ -27243,10 +27240,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="12">
         <v>10</v>
@@ -27393,10 +27390,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="12">
         <v>10</v>
@@ -27545,10 +27542,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" s="12">
         <v>50</v>
@@ -27663,31 +27660,31 @@
         <v>5</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D39" s="12">
         <v>10</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K39" s="12">
         <f>10^-1</f>
@@ -27704,25 +27701,25 @@
         <v>200</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R39" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S39" s="12">
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V39" s="12">
         <v>10.7984432942895</v>
@@ -27731,10 +27728,10 @@
         <v>200</v>
       </c>
       <c r="X39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y39" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z39" s="2"/>
       <c r="AA39" s="12"/>
@@ -27775,31 +27772,31 @@
         <v>6</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="12">
         <v>10</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K40" s="12">
         <f>10^-1</f>
@@ -27816,33 +27813,33 @@
         <v>200</v>
       </c>
       <c r="O40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R40" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S40" s="12">
         <v>7.2900000000000006E-2</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Z40" s="2"/>
       <c r="AA40" s="12"/>
@@ -27883,10 +27880,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D41" s="12">
         <v>10</v>
@@ -27914,16 +27911,16 @@
         <v>0.1</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O41" s="12">
         <f>10^0</f>
@@ -27949,10 +27946,10 @@
         <v>1.65021934868993E-2</v>
       </c>
       <c r="V41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X41" s="12">
         <v>19.077326469266001</v>
@@ -27999,10 +27996,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" s="12">
         <v>10</v>
@@ -28030,16 +28027,16 @@
         <v>0.1</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O42" s="12">
         <f>10^-1</f>
@@ -28065,10 +28062,10 @@
         <v>9.4600703514308097E-5</v>
       </c>
       <c r="V42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W42" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X42" s="12">
         <v>6.9041883127713701</v>
@@ -28112,15 +28109,15 @@
     </row>
     <row r="44" spans="1:48" x14ac:dyDescent="0.3">
       <c r="AN44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A76" s="61" t="s">
-        <v>58</v>
+      <c r="A76" s="95" t="s">
+        <v>57</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D76">
         <f t="shared" ref="D76:Y76" si="47">AVERAGE(LOG10(D7),LOG10(D11),LOG10(D15),LOG10(D19),LOG10(D23))</f>
@@ -28360,9 +28357,9 @@
       </c>
     </row>
     <row r="77" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A77" s="61"/>
+      <c r="A77" s="95"/>
       <c r="B77" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D77">
         <f t="shared" ref="D77:Y77" si="53">AVERAGE(LOG10(D8),LOG10(D12),LOG10(D16),LOG10(D20),LOG10(D24))</f>
@@ -28602,9 +28599,9 @@
       </c>
     </row>
     <row r="78" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A78" s="61"/>
+      <c r="A78" s="95"/>
       <c r="B78" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D78">
         <f t="shared" ref="D78:Y78" si="59">AVERAGE(LOG10(D9),LOG10(D13),LOG10(D17),LOG10(D21),LOG10(D25))</f>
@@ -28844,9 +28841,9 @@
       </c>
     </row>
     <row r="79" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A79" s="61"/>
+      <c r="A79" s="95"/>
       <c r="B79" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D79">
         <f t="shared" ref="D79:Y79" si="64">AVERAGE(LOG10(D10),LOG10(D14),LOG10(D18),LOG10(D22),LOG10(D26))</f>
@@ -29086,11 +29083,11 @@
       </c>
     </row>
     <row r="81" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A81" s="61" t="s">
-        <v>59</v>
+      <c r="A81" s="95" t="s">
+        <v>58</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D81">
         <f t="shared" ref="D81:Y81" si="71">AVEDEV(LOG10(D7),LOG10(D11),LOG10(D15),LOG10(D19),LOG10(D23))</f>
@@ -29330,9 +29327,9 @@
       </c>
     </row>
     <row r="82" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A82" s="61"/>
+      <c r="A82" s="95"/>
       <c r="B82" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D82">
         <f t="shared" ref="D82:Y82" si="77">AVEDEV(LOG10(D8),LOG10(D12),LOG10(D16),LOG10(D20),LOG10(D24))</f>
@@ -29572,9 +29569,9 @@
       </c>
     </row>
     <row r="83" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A83" s="61"/>
+      <c r="A83" s="95"/>
       <c r="B83" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D83">
         <f t="shared" ref="D83:Y83" si="83">AVEDEV(LOG10(D9),LOG10(D13),LOG10(D17),LOG10(D21),LOG10(D25))</f>
@@ -29814,9 +29811,9 @@
       </c>
     </row>
     <row r="84" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A84" s="61"/>
+      <c r="A84" s="95"/>
       <c r="B84" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D84">
         <f t="shared" ref="D84:Y84" si="88">AVEDEV(LOG10(D10),LOG10(D14),LOG10(D18),LOG10(D22),LOG10(D26))</f>
@@ -30059,11 +30056,11 @@
       <c r="B85" s="12"/>
     </row>
     <row r="86" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A86" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B86" s="62" t="s">
-        <v>53</v>
+      <c r="A86" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="B86" s="96" t="s">
+        <v>52</v>
       </c>
       <c r="D86">
         <f t="shared" ref="D86:G86" si="95">POWER(10, D76-D81)</f>
@@ -30303,8 +30300,8 @@
       </c>
     </row>
     <row r="87" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A87" s="61"/>
-      <c r="B87" s="62"/>
+      <c r="A87" s="95"/>
+      <c r="B87" s="96"/>
       <c r="D87">
         <f t="shared" ref="D87:G87" si="102">POWER(10, D76+D81)</f>
         <v>7.3310546557995085E-2</v>
@@ -30543,9 +30540,9 @@
       </c>
     </row>
     <row r="88" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A88" s="61"/>
-      <c r="B88" s="62" t="s">
-        <v>55</v>
+      <c r="A88" s="95"/>
+      <c r="B88" s="96" t="s">
+        <v>54</v>
       </c>
       <c r="D88">
         <f t="shared" ref="D88:G88" si="109">POWER(10, D77-D82)</f>
@@ -30785,8 +30782,8 @@
       </c>
     </row>
     <row r="89" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A89" s="61"/>
-      <c r="B89" s="62"/>
+      <c r="A89" s="95"/>
+      <c r="B89" s="96"/>
       <c r="D89">
         <f t="shared" ref="D89:G89" si="116">POWER(10, D77+D82)</f>
         <v>0.11982771531626747</v>
@@ -31025,9 +31022,9 @@
       </c>
     </row>
     <row r="90" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A90" s="61"/>
-      <c r="B90" s="62" t="s">
-        <v>56</v>
+      <c r="A90" s="95"/>
+      <c r="B90" s="96" t="s">
+        <v>55</v>
       </c>
       <c r="D90">
         <f t="shared" ref="D90:G90" si="123">POWER(10, D78-D83)</f>
@@ -31267,8 +31264,8 @@
       </c>
     </row>
     <row r="91" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A91" s="61"/>
-      <c r="B91" s="62"/>
+      <c r="A91" s="95"/>
+      <c r="B91" s="96"/>
       <c r="D91">
         <f t="shared" ref="D91:G91" si="130">POWER(10, D78+D83)</f>
         <v>0.11982771531626747</v>
@@ -31507,9 +31504,9 @@
       </c>
     </row>
     <row r="92" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A92" s="61"/>
-      <c r="B92" s="62" t="s">
-        <v>54</v>
+      <c r="A92" s="95"/>
+      <c r="B92" s="96" t="s">
+        <v>53</v>
       </c>
       <c r="D92">
         <f t="shared" ref="D92:G92" si="137">POWER(10, D79-D84)</f>
@@ -31749,8 +31746,8 @@
       </c>
     </row>
     <row r="93" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A93" s="61"/>
-      <c r="B93" s="62"/>
+      <c r="A93" s="95"/>
+      <c r="B93" s="96"/>
       <c r="D93">
         <f t="shared" ref="D93:G93" si="144">POWER(10, D79+D84)</f>
         <v>6.1861212555328234E-2</v>
@@ -31989,11 +31986,11 @@
       </c>
     </row>
     <row r="95" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A95" s="61" t="s">
-        <v>61</v>
+      <c r="A95" s="95" t="s">
+        <v>60</v>
       </c>
       <c r="B95" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D95">
         <f t="shared" ref="D95:G95" si="151">D86</f>
@@ -32233,9 +32230,9 @@
       </c>
     </row>
     <row r="96" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A96" s="61"/>
+      <c r="A96" s="95"/>
       <c r="B96" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D96">
         <f t="shared" ref="D96:G96" si="158">D87-D86</f>
@@ -32475,9 +32472,9 @@
       </c>
     </row>
     <row r="97" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A97" s="61"/>
+      <c r="A97" s="95"/>
       <c r="B97" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D97">
         <f t="shared" ref="D97:G102" si="165">D88-D87</f>
@@ -32717,9 +32714,9 @@
       </c>
     </row>
     <row r="98" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A98" s="61"/>
+      <c r="A98" s="95"/>
       <c r="B98" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D98">
         <f t="shared" si="165"/>
@@ -32959,9 +32956,9 @@
       </c>
     </row>
     <row r="99" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A99" s="61"/>
+      <c r="A99" s="95"/>
       <c r="B99" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D99">
         <f t="shared" si="165"/>
@@ -33201,9 +33198,9 @@
       </c>
     </row>
     <row r="100" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A100" s="61"/>
+      <c r="A100" s="95"/>
       <c r="B100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D100">
         <f t="shared" si="165"/>
@@ -33443,9 +33440,9 @@
       </c>
     </row>
     <row r="101" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A101" s="61"/>
+      <c r="A101" s="95"/>
       <c r="B101" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D101">
         <f t="shared" si="165"/>
@@ -33685,9 +33682,9 @@
       </c>
     </row>
     <row r="102" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A102" s="61"/>
+      <c r="A102" s="95"/>
       <c r="B102" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D102">
         <f t="shared" si="165"/>
@@ -33928,6 +33925,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A95:A102"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="A81:A84"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
     <mergeCell ref="AG32:AM32"/>
     <mergeCell ref="AN32:AT32"/>
     <mergeCell ref="BA1:BE1"/>
@@ -33941,23 +33952,9 @@
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="Z32:AF32"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
     <mergeCell ref="G32:R32"/>
     <mergeCell ref="S32:Y32"/>
     <mergeCell ref="B32:F32"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A95:A102"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="A81:A84"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A86:A93"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D6">
     <cfRule type="colorScale" priority="83">
@@ -34716,10 +34713,10 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2">
         <v>-1</v>
@@ -34847,10 +34844,10 @@
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="3">
@@ -35020,7 +35017,7 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -35155,7 +35152,7 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4">
         <v>1.05</v>

</xml_diff>